<commit_message>
Feature: api context; Cleancode
</commit_message>
<xml_diff>
--- a/ait/components/analyze/app/config/mxBase_API_MAP.xlsx
+++ b/ait/components/analyze/app/config/mxBase_API_MAP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\porting_acl\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongyonghan/repos/ait/ait/components/analyze/app/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3E201C-4369-4E9E-9560-FA0B889EB9A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92AFCE2-4951-FE49-AB6B-A3322D8CA22D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mxBase-OpenCVCPU-APIMap" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="307">
   <si>
     <t>昇腾API</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>OpenCV参数</t>
-  </si>
-  <si>
-    <t>对应关系(mxBase:OpenCV)</t>
   </si>
   <si>
     <t>迁移预估人力（人/天）</t>
@@ -5002,10 +4999,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Opencv 4.5.4</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>cv::Mat.size()</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -5126,12 +5119,62 @@
     <t>cv::Mat.rows</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>NV_API</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>昇腾</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>API</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>对应关系</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>(昇腾:NV)</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5211,6 +5254,27 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="HuaweiSans-Bold"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5275,7 +5339,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5343,6 +5407,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5622,29 +5692,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="59.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50.75" style="8" customWidth="1"/>
-    <col min="5" max="6" width="50.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="59.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" style="8" customWidth="1"/>
+    <col min="5" max="6" width="50.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+    <row r="1" spans="1:7" ht="17">
+      <c r="A1" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>276</v>
+        <v>304</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5652,136 +5722,136 @@
       <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="150">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="135">
-      <c r="A2" s="3" t="s">
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="105">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" ht="94.5">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="229.5">
+    <row r="4" spans="1:7" ht="270">
       <c r="A4" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="54">
+    <row r="5" spans="1:7" ht="60">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" ht="256.5">
+    <row r="6" spans="1:7" ht="285">
       <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="G6" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="148.5">
+    <row r="7" spans="1:7" ht="165">
       <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="20" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>30</v>
       </c>
       <c r="G7" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.25">
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>281</v>
-      </c>
       <c r="C8" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="19"/>
@@ -5792,13 +5862,13 @@
     </row>
     <row r="9" spans="1:7" ht="123" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>280</v>
-      </c>
       <c r="C9" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="19"/>
@@ -5807,443 +5877,443 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="135">
+    <row r="10" spans="1:7" ht="150">
       <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="F10" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="G10" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="202.5">
+    <row r="11" spans="1:7" ht="225">
       <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="54">
+    <row r="12" spans="1:7" ht="60">
       <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="148.5">
+    <row r="13" spans="1:7" ht="165">
       <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="409.5">
+    <row r="14" spans="1:7" ht="409.6">
       <c r="A14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="E14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" ht="314">
+      <c r="A15" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>301</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" ht="300">
+      <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="1:7" ht="283.5">
-      <c r="A15" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>303</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:7" ht="270">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="27">
+    <row r="17" spans="1:7" ht="30">
       <c r="A17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="14.25">
+    <row r="18" spans="1:7" ht="15">
       <c r="A18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="14.25">
+    <row r="19" spans="1:7" ht="15">
       <c r="A19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="14.25">
+    <row r="20" spans="1:7" ht="15">
       <c r="A20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="27">
+    <row r="21" spans="1:7" ht="30">
       <c r="A21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:7" ht="27">
+    <row r="22" spans="1:7" ht="30">
       <c r="A22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" ht="27">
+    <row r="23" spans="1:7" ht="30">
       <c r="A23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="14.25">
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" ht="40.5">
+    <row r="25" spans="1:7" ht="45">
       <c r="A25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" ht="27">
+    <row r="26" spans="1:7" ht="30">
       <c r="A26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="17"/>
     </row>
-    <row r="27" spans="1:7" ht="81">
+    <row r="27" spans="1:7" ht="90">
       <c r="A27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="17"/>
     </row>
-    <row r="28" spans="1:7" ht="54">
+    <row r="28" spans="1:7" ht="60">
       <c r="A28" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="17"/>
     </row>
-    <row r="29" spans="1:7" ht="14.25">
+    <row r="29" spans="1:7" ht="15">
       <c r="A29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="17"/>
     </row>
-    <row r="30" spans="1:7" ht="14.25">
+    <row r="30" spans="1:7" ht="15">
       <c r="A30" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="1:7" ht="27">
+    <row r="31" spans="1:7" ht="30">
       <c r="A31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="1:7" ht="54">
+    <row r="32" spans="1:7" ht="60">
       <c r="A32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" ht="27">
+    <row r="33" spans="1:7" ht="30">
       <c r="A33" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" ht="27">
+    <row r="34" spans="1:7" ht="30">
       <c r="A34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" ht="27">
+    <row r="35" spans="1:7" ht="30">
       <c r="A35" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" ht="40.5">
+    <row r="36" spans="1:7" ht="45">
       <c r="A36" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" ht="94.5">
+    <row r="37" spans="1:7" ht="105">
       <c r="A37" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="D37" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -6251,200 +6321,200 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="40.5">
+    <row r="38" spans="1:7" ht="45">
       <c r="A38" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" ht="14.25">
+    <row r="39" spans="1:7" ht="15">
       <c r="A39" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" ht="27">
+    <row r="40" spans="1:7" ht="30">
       <c r="A40" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" ht="27">
+    <row r="41" spans="1:7" ht="30">
       <c r="A41" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="D41" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" ht="27">
+    <row r="42" spans="1:7" ht="30">
       <c r="A42" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>133</v>
-      </c>
       <c r="E42" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" s="15"/>
       <c r="G42" s="17">
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="27">
+    <row r="43" spans="1:7" ht="30">
       <c r="A43" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" ht="14.25">
+    <row r="44" spans="1:7" ht="15">
       <c r="A44" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="E44" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>140</v>
       </c>
       <c r="F44" s="15"/>
       <c r="G44" s="17">
         <v>0.1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="27">
+    <row r="45" spans="1:7" ht="30">
       <c r="A45" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" ht="27">
+    <row r="46" spans="1:7" ht="30">
       <c r="A46" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" ht="40.5">
+    <row r="47" spans="1:7" ht="45">
       <c r="A47" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" ht="54">
+    <row r="48" spans="1:7" ht="60">
       <c r="A48" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" ht="94.5">
+    <row r="49" spans="1:7" ht="105">
       <c r="A49" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="C49" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G49" s="17">
         <v>0.3</v>
@@ -6452,152 +6522,152 @@
     </row>
     <row r="50" spans="1:7" ht="136.5" customHeight="1">
       <c r="A50" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="C50" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E50" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="F50" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>295</v>
       </c>
       <c r="G50" s="17">
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="81">
+    <row r="51" spans="1:7" ht="90">
       <c r="A51" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E51" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>157</v>
-      </c>
       <c r="F51" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G51" s="17">
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="67.5">
+    <row r="52" spans="1:7" ht="75">
       <c r="A52" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="C52" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E52" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="F52" s="15" t="s">
         <v>292</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>294</v>
       </c>
       <c r="G52" s="17">
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="94.5">
+    <row r="53" spans="1:7" ht="105">
       <c r="A53" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="D53" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="E53" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="F53" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="G53" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="121.5">
+    <row r="54" spans="1:7" ht="135">
       <c r="A54" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="D54" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="E54" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="F54" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>169</v>
       </c>
       <c r="G54" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="108">
+    <row r="55" spans="1:7" ht="120">
       <c r="A55" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="D55" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>173</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G55" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="337.5">
+    <row r="56" spans="1:7" ht="384">
       <c r="A56" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="D56" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>178</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
@@ -6605,18 +6675,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="40.5">
+    <row r="57" spans="1:7" ht="45">
       <c r="A57" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="C57" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="D57" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
@@ -6624,41 +6694,41 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="67.5">
+    <row r="58" spans="1:7" ht="75">
       <c r="A58" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="D58" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="E58" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="F58" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>188</v>
       </c>
       <c r="G58" s="17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="54">
+    <row r="59" spans="1:7" ht="60">
       <c r="A59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="D59" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>192</v>
       </c>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
@@ -6666,18 +6736,18 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="121.5">
+    <row r="60" spans="1:7" ht="135">
       <c r="A60" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="D60" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>196</v>
       </c>
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
@@ -6685,45 +6755,45 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="216">
+    <row r="61" spans="1:7" ht="240">
       <c r="A61" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="C61" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="D61" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="E61" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="F61" s="15"/>
       <c r="G61" s="17">
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="27">
+    <row r="62" spans="1:7" ht="30">
       <c r="A62" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="C62" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="D62" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="E62" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="F62" s="16" t="s">
         <v>206</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>207</v>
       </c>
       <c r="G62" s="17">
         <v>0.2</v>
@@ -6748,22 +6818,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="59.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="59.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6771,99 +6841,99 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>276</v>
+        <v>304</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="165">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="148.5">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="94.5">
+    <row r="3" spans="1:7" ht="105">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="256.5">
+    <row r="4" spans="1:7" ht="285">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="105">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="94.5">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>218</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="216">
+    <row r="6" spans="1:7" ht="240">
       <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -6871,12 +6941,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
@@ -6886,16 +6956,16 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="67.5">
+    <row r="8" spans="1:7" ht="75">
       <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -6903,276 +6973,276 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="202.5">
+    <row r="9" spans="1:7" ht="225">
       <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="54">
+    <row r="10" spans="1:7" ht="60">
       <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" ht="81">
+    <row r="11" spans="1:7" ht="90">
       <c r="A11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="135">
+    <row r="12" spans="1:7" ht="150">
       <c r="A12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="300">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="270">
-      <c r="A13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="150">
+      <c r="A14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="135">
-      <c r="A14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="15">
+      <c r="A15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="14.25">
-      <c r="A15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>233</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="14.25">
+    <row r="16" spans="1:7" ht="15">
       <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" ht="14.25">
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="C17" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="27">
+    <row r="18" spans="1:7" ht="30">
       <c r="A18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="C18" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="27">
+    <row r="19" spans="1:7" ht="30">
       <c r="A19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="C19" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="40.5">
+    <row r="20" spans="1:7" ht="45">
       <c r="A20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="F20" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="60">
+      <c r="A21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="B21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" ht="54">
-      <c r="A21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="F21" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="45">
+      <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="B22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" ht="40.5">
-      <c r="A22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="F22" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="30">
+      <c r="A23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" ht="27">
-      <c r="A23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -7180,12 +7250,12 @@
       <c r="F23" s="4"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="14.25">
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -7193,12 +7263,12 @@
       <c r="F24" s="4"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="14.25">
+    <row r="25" spans="1:7" ht="15">
       <c r="A25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -7206,12 +7276,12 @@
       <c r="F25" s="4"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="14.25">
+    <row r="26" spans="1:7" ht="15">
       <c r="A26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -7219,12 +7289,12 @@
       <c r="F26" s="4"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="14.25">
+    <row r="27" spans="1:7" ht="15">
       <c r="A27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -7232,12 +7302,12 @@
       <c r="F27" s="4"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="27">
+    <row r="28" spans="1:7" ht="30">
       <c r="A28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -7245,12 +7315,12 @@
       <c r="F28" s="4"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="54">
+    <row r="29" spans="1:7" ht="60">
       <c r="A29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -7258,12 +7328,12 @@
       <c r="F29" s="4"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="27">
+    <row r="30" spans="1:7" ht="30">
       <c r="A30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -7271,12 +7341,12 @@
       <c r="F30" s="4"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="27">
+    <row r="31" spans="1:7" ht="30">
       <c r="A31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -7284,12 +7354,12 @@
       <c r="F31" s="4"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7" ht="27">
+    <row r="32" spans="1:7" ht="30">
       <c r="A32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -7297,12 +7367,12 @@
       <c r="F32" s="4"/>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:7" ht="40.5">
+    <row r="33" spans="1:7" ht="45">
       <c r="A33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -7310,211 +7380,211 @@
       <c r="F33" s="4"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:7" ht="121.5">
+    <row r="34" spans="1:7" ht="135">
       <c r="A34" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="C34" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>246</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G34" s="7">
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="67.5">
+    <row r="35" spans="1:7" ht="75">
       <c r="A35" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="F35" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="15">
+      <c r="A36" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" ht="14.25">
-      <c r="A36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="C36" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7" ht="27">
+    <row r="37" spans="1:7" ht="30">
       <c r="A37" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="C37" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7" ht="27">
+    <row r="38" spans="1:7" ht="30">
       <c r="A38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:7" ht="27">
+    <row r="39" spans="1:7" ht="30">
       <c r="A39" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="C39" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="27">
+    <row r="40" spans="1:7" ht="30">
       <c r="A40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="C40" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:7" ht="14.25">
+    <row r="41" spans="1:7" ht="15">
       <c r="A41" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="C41" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G41" s="7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="54">
+    <row r="42" spans="1:7" ht="60">
       <c r="A42" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="E42" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="1:7" ht="45">
+      <c r="A43" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G42" s="7"/>
-    </row>
-    <row r="43" spans="1:7" ht="40.5">
-      <c r="A43" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>253</v>
-      </c>
       <c r="D43" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:7" ht="40.5">
+    <row r="44" spans="1:7" ht="45">
       <c r="A44" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -7522,12 +7592,12 @@
       <c r="F44" s="4"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:7" ht="54">
+    <row r="45" spans="1:7" ht="60">
       <c r="A45" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -7535,12 +7605,12 @@
       <c r="F45" s="4"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7" ht="94.5">
+    <row r="46" spans="1:7" ht="105">
       <c r="A46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -7550,12 +7620,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="54">
+    <row r="47" spans="1:7" ht="60">
       <c r="A47" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -7565,55 +7635,55 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="94.5">
+    <row r="48" spans="1:7" ht="105">
       <c r="A48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="C48" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="81">
+    <row r="49" spans="1:7" ht="90">
       <c r="A49" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>165</v>
-      </c>
       <c r="C49" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="54">
+    <row r="50" spans="1:7" ht="60">
       <c r="A50" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="C50" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -7622,15 +7692,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="54">
+    <row r="51" spans="1:7" ht="60">
       <c r="A51" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>176</v>
-      </c>
       <c r="C51" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -7639,15 +7709,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="40.5">
+    <row r="52" spans="1:7" ht="45">
       <c r="A52" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="C52" s="21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -7656,112 +7726,112 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="54">
+    <row r="53" spans="1:7" ht="60">
       <c r="A53" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="C53" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="67.5">
+    <row r="54" spans="1:7" ht="75">
       <c r="A54" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="C54" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>265</v>
-      </c>
       <c r="F54" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G54" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="148.5">
+    <row r="55" spans="1:7" ht="165">
       <c r="A55" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="C55" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>268</v>
-      </c>
       <c r="F55" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G55" s="7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="67.5">
+    <row r="56" spans="1:7" ht="75">
       <c r="A56" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="C56" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="E56" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>271</v>
-      </c>
       <c r="F56" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G56" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="40.5">
+    <row r="57" spans="1:7" ht="45">
       <c r="A57" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>203</v>
-      </c>
       <c r="C57" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>273</v>
-      </c>
       <c r="F57" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G57" s="7">
         <v>0.2</v>
@@ -7787,21 +7857,10 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="1"/>
-  <pixelatorList sheetStid="3"/>
-  <pixelatorList sheetStid="4"/>
-</pixelators>
+<autofilters xmlns="https://web.wps.cn/et/2018/main"/>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
-  <rangeList sheetStid="1" master=""/>
-  <rangeList sheetStid="3" master=""/>
-</allowEditUser>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
     <woSheetProps sheetStid="1" interlineOnOff="0" interlineColor="0" isDbSheet="0"/>
@@ -7813,8 +7872,19 @@
 </woProps>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
+  <rangeList sheetStid="1" master=""/>
+  <rangeList sheetStid="3" master=""/>
+</allowEditUser>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<autofilters xmlns="https://web.wps.cn/et/2018/main"/>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="1"/>
+  <pixelatorList sheetStid="3"/>
+  <pixelatorList sheetStid="4"/>
+</pixelators>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7827,7 +7897,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5662047-3127-477A-AC3A-1D340467FB41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
@@ -7836,6 +7906,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
@@ -7844,17 +7923,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5662047-3127-477A-AC3A-1D340467FB41}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>

</xml_diff>